<commit_message>
Config Edited Aug 30
</commit_message>
<xml_diff>
--- a/Motivational story/Config.xlsx
+++ b/Motivational story/Config.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -24,15 +24,9 @@
     <t>Value</t>
   </si>
   <si>
-    <t>Password</t>
-  </si>
-  <si>
     <t>Fromaddress</t>
   </si>
   <si>
-    <t>sharon4199</t>
-  </si>
-  <si>
     <t>Toaddress</t>
   </si>
   <si>
@@ -64,6 +58,9 @@
   </si>
   <si>
     <t>HtmlStyle</t>
+  </si>
+  <si>
+    <t>rpapilotbots@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;html&gt;
@@ -76,23 +73,20 @@
 &lt;h3&gt;Moral of the Story&lt;/h3&gt;
 &lt;p&gt;{2}&lt;/p&gt;&lt;/br&gt;
 &lt;p&gt;Thanks and Regards&lt;/p&gt;&lt;/br&gt;
-&lt;p&gt;Sharon Gifta G&lt;/p&gt;
+&lt;p&gt;Smartbots Team&lt;/p&gt;
 &lt;/body&gt;
 &lt;/html&gt;
 </t>
   </si>
   <si>
-    <t>sankaravenie5@gmail.com;aartiak.e5@gmail.com;narenbagavathye5@gmail.com;sharongiftae5@gmail.com;prasanth9534@gmail.com;sathyamoorthie5@gmail.com;sornalakshmie5@gmail.com;alagappan.m@e5.ai;naresh.kumar@e5.ai;muthukumarsekar1986@gmail.com;lakshmi.u@tiliconveli.com</t>
-  </si>
-  <si>
-    <t>rpapilotbots@gmail.com</t>
+    <t>sankaravenie5@gmail.com;aartiak.e5@gmail.com;narenbagavathye5@gmail.com;sharongiftae5@gmail.com;prasanth9534@gmail.com;sathyamoorthie5@gmail.com;sornalakshmie5@gmail.com;naresh.kumar@e5.ai;lakshmi.u@tiliconveli.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,6 +232,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -272,6 +267,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -447,20 +443,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.85546875" customWidth="1"/>
     <col min="2" max="2" width="118" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -468,104 +464,96 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="45">
-      <c r="A4" t="s">
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="B5">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="225">
-      <c r="A9" t="s">
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="B10" s="1"/>
-    </row>
-    <row r="13" spans="1:2">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="B14" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B4" display="sankaravenie5@gmail.com;aartiak.e5@gmail.com;narenbagavathye5@gmail.com;sharongiftae5@gmail.com;prasanth9534@gmail.com;sathyamoorthie5@gmail.com;sornalakshmie5@gmail.com;alagappan.m@e5.ai;naresh.kumar@e5.ai;muthukumarsekar1986@gmail.com;lakshmi.u@tiliconv"/>
+    <hyperlink ref="B3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -579,20 +567,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.140625" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -600,12 +588,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>